<commit_message>
The app was updated to have a  face recognition after taking a  photograph of the user who needed to access the Gym, plus this new code contain cool interface for this
The app was updated to have a  face recognition after taking a  photograph of the user who needed to access the Gym, plus this new code contain cool interface for this
</commit_message>
<xml_diff>
--- a/attendance/attendance.xlsx
+++ b/attendance/attendance.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,72 +441,79 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Date</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Count</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>First Seen Time</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Last Seen Time</t>
+          <t>Image_Path</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Yesen</t>
+          <t>Malindha</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2024-07-26</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>33</v>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>21:13:24</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>21:33:33</t>
+          <t>person2.jpg</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Malindha</t>
+          <t>Lalithya</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2024-07-26</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>5</v>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>21:33:22</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>21:33:35</t>
+          <t>person3.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Anuradha</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>person-4.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Malinga</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>person6.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Hasith</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>person8.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>0012</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>0012.jpg</t>
         </is>
       </c>
     </row>

</xml_diff>